<commit_message>
Generated new outjob files
</commit_message>
<xml_diff>
--- a/CTS-SAT-1 Onboard Computer/Project Outputs for OBC Development Board/BOM/Bill of Materials-OBC Development Board.xlsx
+++ b/CTS-SAT-1 Onboard Computer/Project Outputs for OBC Development Board/BOM/Bill of Materials-OBC Development Board.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anush\Documents\GitHub\CTS-SAT-1-OBC-PCB\CTS-SAT-1 Onboard Computer\Project Outputs for OBC Development Board\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CFB14CB8-7212-4B6E-A338-369EAA8C18EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D10A3F3-4378-4300-BE33-4E3AB34FE921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="8880" xr2:uid="{4E051976-E250-41AF-8193-313DB41BBFBB}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A955719F-2178-4D4E-95C0-AF25EA44656D}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-OBC Developme" sheetId="1" r:id="rId1"/>
@@ -18,20 +18,28 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Bill of Materials-OBC Developme'!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="187">
-  <si>
-    <t>Line #</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="217">
   <si>
     <t>Name</t>
   </si>
@@ -42,45 +50,33 @@
     <t>Designator</t>
   </si>
   <si>
+    <t>Footprint</t>
+  </si>
+  <si>
+    <t>LibRef</t>
+  </si>
+  <si>
     <t>Quantity</t>
   </si>
   <si>
-    <t>Distributor</t>
-  </si>
-  <si>
-    <t>DesignItemId</t>
-  </si>
-  <si>
-    <t>Manufacturer 1</t>
-  </si>
-  <si>
-    <t>Manufacturer Part Number 1</t>
-  </si>
-  <si>
-    <t>Manufacturer Lifecycle 1</t>
-  </si>
-  <si>
-    <t>Supplier 1</t>
-  </si>
-  <si>
-    <t>Supplier Part Number 1</t>
-  </si>
-  <si>
-    <t>Supplier Unit Price 1</t>
-  </si>
-  <si>
-    <t>Supplier Subtotal 1</t>
+    <t>Manufacturer Part #</t>
+  </si>
+  <si>
+    <t>Manfacturer Part #</t>
+  </si>
+  <si>
+    <t>PC104 Mounting</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>PC104 Mounting</t>
-  </si>
-  <si>
     <t>*1, *2, *3, *4</t>
   </si>
   <si>
+    <t>PC104 Mounting Points</t>
+  </si>
+  <si>
     <t>0.1uF</t>
   </si>
   <si>
@@ -90,12 +86,15 @@
     <t>C1, C3, C4, C5, C6, C7, C8, C9, C10, C12, C14, C15, C16, C17, C18, C19, C20, C22, C23, C24, C25, C26, C27, C28, C29, C30, C32, C51, C52, C53, C54</t>
   </si>
   <si>
-    <t>LCSC</t>
+    <t>0603</t>
   </si>
   <si>
     <t>CC-100nF-25V-X7R-0603</t>
   </si>
   <si>
+    <t>GCJ188R71E104KA12D</t>
+  </si>
+  <si>
     <t>1uF</t>
   </si>
   <si>
@@ -105,12 +104,12 @@
     <t>C2, C31</t>
   </si>
   <si>
-    <t>Digikey</t>
-  </si>
-  <si>
     <t>CC-105-K-25V-X7R-0603</t>
   </si>
   <si>
+    <t>CC0603KRX7R8BB105</t>
+  </si>
+  <si>
     <t>4.7uF</t>
   </si>
   <si>
@@ -120,9 +119,15 @@
     <t>C11, C13, C48, C49, C50</t>
   </si>
   <si>
+    <t>CAP TANT 1206 (A) TCJ</t>
+  </si>
+  <si>
     <t>CT-474-M-20V-OTH-1206</t>
   </si>
   <si>
+    <t>TAJA475K020RNJ</t>
+  </si>
+  <si>
     <t>15 pF</t>
   </si>
   <si>
@@ -132,15 +137,18 @@
     <t>C21</t>
   </si>
   <si>
+    <t>0402</t>
+  </si>
+  <si>
     <t>CC-159-J-50V-C0G-0402</t>
   </si>
   <si>
+    <t>CC0402FRNPO9BN150</t>
+  </si>
+  <si>
     <t>22uF</t>
   </si>
   <si>
-    <t>22uF 25V  ±10% 1.4Ω 2312  SMD Tantalum Capacitor, TAJC226K025RNJ</t>
-  </si>
-  <si>
     <t>C33</t>
   </si>
   <si>
@@ -156,6 +164,9 @@
     <t>C34, C35, C36</t>
   </si>
   <si>
+    <t>FP-GRM32E-0_3-0_2-MFG</t>
+  </si>
+  <si>
     <t>CMP-2000-06360-2, CC-GRM32ER60J476ME20L</t>
   </si>
   <si>
@@ -168,6 +179,9 @@
     <t>CC-104-K-25V-X7R-0402</t>
   </si>
   <si>
+    <t>CC0402KPX7R8BB104</t>
+  </si>
+  <si>
     <t>0.7 pF</t>
   </si>
   <si>
@@ -180,6 +194,9 @@
     <t>CC-710-K-50V-X7R-0603</t>
   </si>
   <si>
+    <t>CBR06C708B5GAC</t>
+  </si>
+  <si>
     <t>100pF</t>
   </si>
   <si>
@@ -192,6 +209,9 @@
     <t>CC-104-K-25V-X5R-0402</t>
   </si>
   <si>
+    <t>CC0603KRX7R9BB101</t>
+  </si>
+  <si>
     <t>33 pF</t>
   </si>
   <si>
@@ -204,6 +224,9 @@
     <t>CC-339-K-50V-X7R-0603</t>
   </si>
   <si>
+    <t>C0603C330K5RAC7867</t>
+  </si>
+  <si>
     <t>4.7 µF</t>
   </si>
   <si>
@@ -213,6 +236,9 @@
     <t>C44</t>
   </si>
   <si>
+    <t>GRM188Z71C475KE21J</t>
+  </si>
+  <si>
     <t>D-SML-D12U1WT86</t>
   </si>
   <si>
@@ -222,6 +248,9 @@
     <t>D1, D2, D3, D4, D5, D6</t>
   </si>
   <si>
+    <t>SML-D12U1WT86</t>
+  </si>
+  <si>
     <t>B540C-13-F</t>
   </si>
   <si>
@@ -243,6 +272,9 @@
     <t>J1, J2, J19, J21</t>
   </si>
   <si>
+    <t>TSW-106-05-T-S</t>
+  </si>
+  <si>
     <t>J-0532610871</t>
   </si>
   <si>
@@ -252,7 +284,10 @@
     <t>J3, J8, J12</t>
   </si>
   <si>
-    <t>Digi-Key</t>
+    <t>J-532610871</t>
+  </si>
+  <si>
+    <t>0532610871</t>
   </si>
   <si>
     <t>J-0532610471</t>
@@ -264,6 +299,12 @@
     <t>J4, J14, J15</t>
   </si>
   <si>
+    <t>J-53261-0471</t>
+  </si>
+  <si>
+    <t>0532610471</t>
+  </si>
+  <si>
     <t>J-ESQ-126-14-G-D</t>
   </si>
   <si>
@@ -273,6 +314,9 @@
     <t>J5, J6</t>
   </si>
   <si>
+    <t>ESQ-126-14-G-D</t>
+  </si>
+  <si>
     <t>J-0532610671</t>
   </si>
   <si>
@@ -282,6 +326,9 @@
     <t>J7, J11</t>
   </si>
   <si>
+    <t>0532610671</t>
+  </si>
+  <si>
     <t>J9</t>
   </si>
   <si>
@@ -294,6 +341,9 @@
     <t>J10, J13</t>
   </si>
   <si>
+    <t>0530471010</t>
+  </si>
+  <si>
     <t>252105</t>
   </si>
   <si>
@@ -318,6 +368,9 @@
     <t>L-IHLP4040DZER6R8M01</t>
   </si>
   <si>
+    <t>IHLP4040DZER6R8M01</t>
+  </si>
+  <si>
     <t>220R</t>
   </si>
   <si>
@@ -330,6 +383,9 @@
     <t>RT-220R-F-1/16W-0603</t>
   </si>
   <si>
+    <t>RR0816P-221-D</t>
+  </si>
+  <si>
     <t>0R</t>
   </si>
   <si>
@@ -342,6 +398,9 @@
     <t>RT-0R00-F-1/10W-0603</t>
   </si>
   <si>
+    <t>RMCF0603ZT0R00</t>
+  </si>
+  <si>
     <t>1K</t>
   </si>
   <si>
@@ -354,6 +413,9 @@
     <t>RT-1K0-F-1/16W-0603</t>
   </si>
   <si>
+    <t>CPF0603F1K0C1</t>
+  </si>
+  <si>
     <t>22R</t>
   </si>
   <si>
@@ -366,6 +428,9 @@
     <t>RT-22R0-F-1/16W-0603</t>
   </si>
   <si>
+    <t>RR0816Q-220-D</t>
+  </si>
+  <si>
     <t>4K7</t>
   </si>
   <si>
@@ -378,6 +443,9 @@
     <t>RT-4K7-F-1/16W-0603</t>
   </si>
   <si>
+    <t>CR0603-FX-4701ELF</t>
+  </si>
+  <si>
     <t>0R33</t>
   </si>
   <si>
@@ -387,10 +455,13 @@
     <t>R33</t>
   </si>
   <si>
+    <t>2512</t>
+  </si>
+  <si>
     <t>RT-0R33-F-4W-2512</t>
   </si>
   <si>
-    <t>4423-VMS-R330-1.0-UCT-ND</t>
+    <t>VMS-R330-1.0-U</t>
   </si>
   <si>
     <t>10K</t>
@@ -405,12 +476,18 @@
     <t>RT-10K0-F-1/16W-0603</t>
   </si>
   <si>
+    <t>CPF0603B10KE</t>
+  </si>
+  <si>
     <t>RES 10K OHM 1% 1/8W 0603</t>
   </si>
   <si>
     <t>R60, R61, R83</t>
   </si>
   <si>
+    <t>RNCP0603FTD10K0</t>
+  </si>
+  <si>
     <t>100R</t>
   </si>
   <si>
@@ -423,6 +500,9 @@
     <t>RT-100R-F-1/16W-0603</t>
   </si>
   <si>
+    <t>RR08P100DCT-ND</t>
+  </si>
+  <si>
     <t>S-KH-6X6X4.3H-STM</t>
   </si>
   <si>
@@ -432,6 +512,9 @@
     <t>S1</t>
   </si>
   <si>
+    <t>KH-6X6X4.3H-STM</t>
+  </si>
+  <si>
     <t>TP</t>
   </si>
   <si>
@@ -450,7 +533,7 @@
     <t>U1</t>
   </si>
   <si>
-    <t>Mouser</t>
+    <t>STM32L4R5ZIT6</t>
   </si>
   <si>
     <t>S70FL01GSAGMFI011</t>
@@ -510,6 +593,9 @@
     <t>U9</t>
   </si>
   <si>
+    <t>MAX3378EEUD+T</t>
+  </si>
+  <si>
     <t>MAX3086EESD+T</t>
   </si>
   <si>
@@ -543,6 +629,9 @@
     <t>U13</t>
   </si>
   <si>
+    <t>HMC544AETR</t>
+  </si>
+  <si>
     <t>SN74LVC1G14DCKR</t>
   </si>
   <si>
@@ -564,6 +653,9 @@
     <t>U15</t>
   </si>
   <si>
+    <t>MSOP-8_STM-M</t>
+  </si>
+  <si>
     <t>U-STDS75DS2F</t>
   </si>
   <si>
@@ -589,6 +681,15 @@
   </si>
   <si>
     <t>Y-TG-3541CE 32.7680KXB3</t>
+  </si>
+  <si>
+    <t>22uF 25V  ±10% 1.4Ω 2312  SMD Tantalum Capacitor</t>
+  </si>
+  <si>
+    <t>TAJC226K025RNJ</t>
+  </si>
+  <si>
+    <t>'0532610671</t>
   </si>
 </sst>
 </file>
@@ -599,7 +700,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -679,39 +780,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="E97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="196B24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -763,7 +864,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -874,13 +975,6 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -889,6 +983,13 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -953,41 +1054,53 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43FE66A6-E010-4DBB-B49B-D6E294B96A3B}">
-  <dimension ref="A1:N48"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17CCFE7E-ECBB-447F-ABB1-3D9513BEAC5B}">
+  <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" customWidth="1"/>
-    <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="35.33203125" customWidth="1"/>
-    <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" customWidth="1"/>
-    <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="15.77734375" customWidth="1"/>
-    <col min="9" max="9" width="26" customWidth="1"/>
-    <col min="10" max="10" width="22.33203125" customWidth="1"/>
-    <col min="11" max="11" width="11.77734375" customWidth="1"/>
-    <col min="12" max="12" width="21.77734375" customWidth="1"/>
-    <col min="13" max="13" width="19.33203125" customWidth="1"/>
-    <col min="14" max="14" width="18.44140625" customWidth="1"/>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="2" max="2" width="144.21875" customWidth="1"/>
+    <col min="3" max="6" width="19" customWidth="1"/>
+    <col min="7" max="8" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1012,202 +1125,152 @@
       <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="1">
-        <v>4</v>
-      </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="2" t="s">
+      <c r="F3" s="1">
+        <v>31</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="1">
+      <c r="E4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="1">
+        <v>5</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="1">
-        <v>2</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="1">
-        <v>5</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6" s="1">
         <v>1</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="B7" s="2" t="s">
-        <v>35</v>
+        <v>214</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F7" s="1">
         <v>1</v>
       </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>39</v>
@@ -1218,1214 +1281,980 @@
       <c r="D8" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="1">
         <v>3</v>
       </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="2" t="s">
-        <v>42</v>
-      </c>
+      <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" s="1">
+        <v>32</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="1">
         <v>1</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="G9" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" s="1">
+        <v>15</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="1">
         <v>2</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="G10" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E11" s="1">
+        <v>15</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="1">
         <v>3</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="G11" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>14</v>
+        <v>57</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E12" s="1">
+        <v>15</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F12" s="1">
         <v>2</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="G12" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E13" s="1">
+        <v>15</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="1">
         <v>1</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="G13" s="2" t="s">
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E14" s="1">
+        <v>66</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F14" s="1">
         <v>6</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="G14" s="2" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E15" s="1">
+        <v>73</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F15" s="1">
         <v>1</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="G15" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E16" s="1">
+        <v>74</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F16" s="1">
         <v>4</v>
       </c>
-      <c r="F16" s="1"/>
       <c r="G16" s="2" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E17" s="1">
+        <v>81</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F17" s="1">
         <v>3</v>
       </c>
-      <c r="F17" s="2" t="s">
-        <v>74</v>
-      </c>
       <c r="G17" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>14</v>
+        <v>83</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E18" s="1">
+        <v>86</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F18" s="1">
         <v>3</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>74</v>
-      </c>
       <c r="G18" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>14</v>
+        <v>88</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E19" s="1">
+        <v>88</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F19" s="1">
         <v>2</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="G19" s="2" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>14</v>
+        <v>92</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E20" s="1">
+        <v>92</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F20" s="1">
         <v>2</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G20" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>14</v>
+        <v>92</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E21" s="1">
+        <v>92</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F21" s="1">
         <v>1</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G21" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>14</v>
+        <v>97</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E22" s="1">
+        <v>97</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F22" s="1">
         <v>2</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="G22" s="2" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>14</v>
+        <v>101</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E23" s="1">
+        <v>104</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F23" s="1">
         <v>4</v>
       </c>
-      <c r="F23" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="G23" s="2" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>14</v>
+        <v>105</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E24" s="1">
+        <v>108</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F24" s="1">
         <v>1</v>
       </c>
-      <c r="F24" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="G24" s="2" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>14</v>
+        <v>110</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E25" s="1">
+        <v>15</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F25" s="1">
         <v>5</v>
       </c>
-      <c r="F25" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="G25" s="2" t="s">
-        <v>99</v>
+        <v>114</v>
       </c>
       <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>14</v>
+        <v>115</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="E26" s="1">
+        <v>15</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F26" s="1">
         <v>35</v>
       </c>
-      <c r="F26" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="G26" s="2" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-      <c r="N26" s="1"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>14</v>
+        <v>120</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>104</v>
+        <v>121</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>105</v>
+        <v>122</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E27" s="1">
+        <v>15</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F27" s="1">
         <v>3</v>
       </c>
-      <c r="F27" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="G27" s="2" t="s">
-        <v>107</v>
+        <v>124</v>
       </c>
       <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
-      <c r="N27" s="1"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>14</v>
+        <v>125</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>108</v>
+        <v>126</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>109</v>
+        <v>127</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E28" s="1">
+        <v>15</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F28" s="1">
         <v>33</v>
       </c>
-      <c r="F28" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="G28" s="2" t="s">
-        <v>111</v>
+        <v>129</v>
       </c>
       <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
-      <c r="N28" s="1"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>14</v>
+        <v>130</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>113</v>
+        <v>132</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E29" s="1">
+        <v>15</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F29" s="1">
         <v>12</v>
       </c>
-      <c r="F29" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="G29" s="2" t="s">
-        <v>115</v>
+        <v>134</v>
       </c>
       <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
-      <c r="N29" s="1"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A30" s="1"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>135</v>
+      </c>
       <c r="B30" s="2" t="s">
-        <v>116</v>
+        <v>136</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>117</v>
+        <v>137</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="E30" s="1">
+        <v>138</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F30" s="1">
         <v>1</v>
       </c>
-      <c r="F30" s="1"/>
       <c r="G30" s="2" t="s">
-        <v>119</v>
+        <v>140</v>
       </c>
       <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L30" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="M30" s="1"/>
-      <c r="N30" s="1"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>14</v>
+        <v>141</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>121</v>
+        <v>142</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>122</v>
+        <v>143</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="E31" s="1">
+        <v>15</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F31" s="1">
         <v>11</v>
       </c>
-      <c r="F31" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="G31" s="2" t="s">
-        <v>124</v>
+        <v>145</v>
       </c>
       <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
-      <c r="L31" s="1"/>
-      <c r="M31" s="1"/>
-      <c r="N31" s="1"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>14</v>
+        <v>141</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>121</v>
+        <v>146</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>125</v>
+        <v>147</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E32" s="1">
+        <v>15</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F32" s="1">
         <v>3</v>
       </c>
-      <c r="F32" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="G32" s="2" t="s">
-        <v>124</v>
+        <v>148</v>
       </c>
       <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
-      <c r="L32" s="1"/>
-      <c r="M32" s="1"/>
-      <c r="N32" s="1"/>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>14</v>
+        <v>149</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>127</v>
+        <v>150</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>128</v>
+        <v>151</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E33" s="1">
+        <v>15</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F33" s="1">
         <v>2</v>
       </c>
-      <c r="F33" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="G33" s="2" t="s">
-        <v>130</v>
+        <v>153</v>
       </c>
       <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
-      <c r="L33" s="1"/>
-      <c r="M33" s="1"/>
-      <c r="N33" s="1"/>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>14</v>
+        <v>154</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>131</v>
+        <v>155</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>132</v>
+        <v>156</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E34" s="1">
+        <v>154</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F34" s="1">
         <v>1</v>
       </c>
-      <c r="F34" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="G34" s="2" t="s">
-        <v>131</v>
+        <v>157</v>
       </c>
       <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
-      <c r="N34" s="1"/>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>14</v>
+        <v>158</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>134</v>
+        <v>159</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>135</v>
+        <v>160</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="E35" s="1">
+        <v>158</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F35" s="1">
         <v>2</v>
       </c>
-      <c r="F35" s="1"/>
-      <c r="G35" s="2" t="s">
-        <v>134</v>
-      </c>
+      <c r="G35" s="1"/>
       <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
-      <c r="L35" s="1"/>
-      <c r="M35" s="1"/>
-      <c r="N35" s="1"/>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>14</v>
+        <v>161</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>137</v>
+        <v>162</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>138</v>
+        <v>163</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="E36" s="1">
+        <v>161</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="F36" s="1">
         <v>1</v>
       </c>
-      <c r="F36" s="2" t="s">
-        <v>140</v>
-      </c>
       <c r="G36" s="2" t="s">
-        <v>137</v>
+        <v>164</v>
       </c>
       <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-      <c r="K36" s="1"/>
-      <c r="L36" s="1"/>
-      <c r="M36" s="1"/>
-      <c r="N36" s="1"/>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>14</v>
+        <v>165</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>141</v>
+        <v>166</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>142</v>
+        <v>167</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="E37" s="1">
+        <v>168</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F37" s="1">
         <v>2</v>
       </c>
-      <c r="F37" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="G37" s="2" t="s">
-        <v>144</v>
+        <v>165</v>
       </c>
       <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
-      <c r="L37" s="1"/>
-      <c r="M37" s="1"/>
-      <c r="N37" s="1"/>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>14</v>
+        <v>169</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>145</v>
+        <v>170</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>146</v>
+        <v>171</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="E38" s="1">
+        <v>172</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="F38" s="1">
         <v>2</v>
       </c>
-      <c r="F38" s="1"/>
       <c r="G38" s="2" t="s">
-        <v>148</v>
+        <v>169</v>
       </c>
       <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
-      <c r="L38" s="1"/>
-      <c r="M38" s="1"/>
-      <c r="N38" s="1"/>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>14</v>
+        <v>173</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>149</v>
+        <v>174</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>150</v>
+        <v>175</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="E39" s="1">
+        <v>176</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="F39" s="1">
         <v>1</v>
       </c>
-      <c r="F39" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="G39" s="2" t="s">
-        <v>152</v>
+        <v>173</v>
       </c>
       <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-      <c r="K39" s="1"/>
-      <c r="L39" s="1"/>
-      <c r="M39" s="1"/>
-      <c r="N39" s="1"/>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>14</v>
+        <v>177</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>153</v>
+        <v>178</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>154</v>
+        <v>179</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="E40" s="1">
+        <v>180</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="F40" s="1">
         <v>2</v>
       </c>
-      <c r="F40" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="G40" s="2" t="s">
-        <v>156</v>
+        <v>177</v>
       </c>
       <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
-      <c r="K40" s="1"/>
-      <c r="L40" s="1"/>
-      <c r="M40" s="1"/>
-      <c r="N40" s="1"/>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>14</v>
+        <v>181</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>157</v>
+        <v>182</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>158</v>
+        <v>183</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="E41" s="1">
+        <v>181</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="F41" s="1">
         <v>1</v>
       </c>
-      <c r="F41" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="G41" s="2" t="s">
-        <v>157</v>
+        <v>184</v>
       </c>
       <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-      <c r="K41" s="1"/>
-      <c r="L41" s="1"/>
-      <c r="M41" s="1"/>
-      <c r="N41" s="1"/>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>14</v>
+        <v>185</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>160</v>
+        <v>186</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>161</v>
+        <v>187</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="E42" s="1">
+        <v>188</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="F42" s="1">
         <v>1</v>
       </c>
-      <c r="F42" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="G42" s="2" t="s">
-        <v>163</v>
+        <v>185</v>
       </c>
       <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-      <c r="K42" s="1"/>
-      <c r="L42" s="1"/>
-      <c r="M42" s="1"/>
-      <c r="N42" s="1"/>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>14</v>
+        <v>189</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>164</v>
+        <v>190</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>165</v>
+        <v>191</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="E43" s="1">
+        <v>192</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="F43" s="1">
         <v>1</v>
       </c>
-      <c r="F43" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="G43" s="2" t="s">
-        <v>167</v>
+        <v>189</v>
       </c>
       <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
-      <c r="J43" s="1"/>
-      <c r="K43" s="1"/>
-      <c r="L43" s="1"/>
-      <c r="M43" s="1"/>
-      <c r="N43" s="1"/>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>14</v>
+        <v>193</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>168</v>
+        <v>194</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>169</v>
+        <v>195</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="E44" s="1">
+        <v>193</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F44" s="1">
         <v>1</v>
       </c>
-      <c r="F44" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="G44" s="2" t="s">
-        <v>168</v>
+        <v>196</v>
       </c>
       <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
-      <c r="K44" s="1"/>
-      <c r="L44" s="1"/>
-      <c r="M44" s="1"/>
-      <c r="N44" s="1"/>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>14</v>
+        <v>197</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>171</v>
+        <v>198</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>172</v>
+        <v>199</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="E45" s="1">
+        <v>200</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="F45" s="1">
         <v>1</v>
       </c>
-      <c r="F45" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="G45" s="2" t="s">
-        <v>174</v>
+        <v>197</v>
       </c>
       <c r="H45" s="1"/>
-      <c r="I45" s="1"/>
-      <c r="J45" s="1"/>
-      <c r="K45" s="1"/>
-      <c r="L45" s="1"/>
-      <c r="M45" s="1"/>
-      <c r="N45" s="1"/>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>14</v>
+        <v>201</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>175</v>
+        <v>202</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>176</v>
+        <v>203</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="E46" s="1">
+        <v>204</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="F46" s="1">
         <v>1</v>
       </c>
-      <c r="F46" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="G46" s="2" t="s">
-        <v>178</v>
+        <v>201</v>
       </c>
       <c r="H46" s="1"/>
-      <c r="I46" s="1"/>
-      <c r="J46" s="1"/>
-      <c r="K46" s="1"/>
-      <c r="L46" s="1"/>
-      <c r="M46" s="1"/>
-      <c r="N46" s="1"/>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>14</v>
+        <v>206</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>179</v>
+        <v>207</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>180</v>
+        <v>208</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="E47" s="1">
+        <v>209</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="F47" s="1">
         <v>1</v>
       </c>
-      <c r="F47" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="G47" s="2" t="s">
-        <v>182</v>
+        <v>206</v>
       </c>
       <c r="H47" s="1"/>
-      <c r="I47" s="1"/>
-      <c r="J47" s="1"/>
-      <c r="K47" s="1"/>
-      <c r="L47" s="1"/>
-      <c r="M47" s="1"/>
-      <c r="N47" s="1"/>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>14</v>
+        <v>210</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>183</v>
+        <v>211</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>184</v>
+        <v>212</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="E48" s="1">
+        <v>213</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="F48" s="1">
         <v>1</v>
       </c>
-      <c r="F48" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="G48" s="2" t="s">
-        <v>186</v>
+        <v>210</v>
       </c>
       <c r="H48" s="1"/>
-      <c r="I48" s="1"/>
-      <c r="J48" s="1"/>
-      <c r="K48" s="1"/>
-      <c r="L48" s="1"/>
-      <c r="M48" s="1"/>
-      <c r="N48" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>